<commit_message>
fix frequency and magnitude error
</commit_message>
<xml_diff>
--- a/data/Phil_DB.xlsx
+++ b/data/Phil_DB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\GCRF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\GCRF\figure\gcrf-figure\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2564213-588E-435A-A7DF-EC7FD63DB001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119E2238-EFE6-488E-99EC-1BE2B7AE9647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flooding" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Earthquake" sheetId="3" r:id="rId3"/>
     <sheet name="Meteorology" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -7295,7 +7295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9009,7 +9011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+    <sheetView topLeftCell="A169" workbookViewId="0">
       <selection activeCell="P176" sqref="P176"/>
     </sheetView>
   </sheetViews>

</xml_diff>